<commit_message>
QC script through with species and length corrections
</commit_message>
<xml_diff>
--- a/FishLandings/data/Action_required_species_list.xlsx
+++ b/FishLandings/data/Action_required_species_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Kenya_SamakiSalama/FishLandings/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CE91DE-E418-C94C-9F8A-EEA780B05E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331EF3CD-2D18-4045-8A37-DCB18CD8B9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="19700" activeTab="2" xr2:uid="{8E5BDA33-4AD9-5F43-B652-B251EBD6C2CD}"/>
   </bookViews>
@@ -2454,7 +2454,7 @@
   <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>